<commit_message>
Fix: added start script for Render backend
</commit_message>
<xml_diff>
--- a/server/invoices.xlsx
+++ b/server/invoices.xlsx
@@ -3,6 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+  </bookViews>
   <sheets>
     <sheet sheetId="1" name="Invoices" state="visible" r:id="rId4"/>
   </sheets>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t>Invoice No</t>
   </si>
@@ -121,28 +124,31 @@
     <t>2000</t>
   </si>
   <si>
-    <t>222</t>
-  </si>
-  <si>
-    <t>JEYABRAKASAN</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>11-002</t>
-  </si>
-  <si>
-    <t>line follower, maze</t>
-  </si>
-  <si>
-    <t>2, 3</t>
-  </si>
-  <si>
-    <t>1000, 1000</t>
+    <t>11-004</t>
+  </si>
+  <si>
+    <t>23.11.2025</t>
+  </si>
+  <si>
+    <t>dhanush</t>
+  </si>
+  <si>
+    <t>dhanushh@gamil</t>
+  </si>
+  <si>
+    <t>fireworks</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>877</t>
+  </si>
+  <si>
+    <t>432</t>
   </si>
 </sst>
 </file>
@@ -519,8 +525,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O10"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -806,13 +817,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -821,31 +832,31 @@
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J7">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="K7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L7">
         <v>200</v>
       </c>
       <c r="M7">
-        <v>4000</v>
+        <v>3100</v>
       </c>
       <c r="N7">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="O7">
         <v>3000</v>
@@ -853,60 +864,60 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J8">
-        <v>400000</v>
+        <v>3000</v>
       </c>
       <c r="K8">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="L8">
-        <v>4000</v>
+        <v>200</v>
       </c>
       <c r="M8">
-        <v>397000</v>
+        <v>3100</v>
       </c>
       <c r="N8">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="O8">
-        <v>387000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -915,81 +926,34 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
         <v>41</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>42</v>
       </c>
-      <c r="I9" t="s">
-        <v>43</v>
-      </c>
       <c r="J9">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="K9">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="L9">
         <v>200</v>
       </c>
       <c r="M9">
-        <v>5000</v>
+        <v>3100</v>
       </c>
       <c r="N9">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="O9">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10">
-        <v>5000</v>
-      </c>
-      <c r="K10">
-        <v>200</v>
-      </c>
-      <c r="L10">
-        <v>200</v>
-      </c>
-      <c r="M10">
-        <v>5000</v>
-      </c>
-      <c r="N10">
-        <v>1000</v>
-      </c>
-      <c r="O10">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>